<commit_message>
Applied css style changes to numerical and spoken link name testing.
</commit_message>
<xml_diff>
--- a/Iteration 2/Survey/Survey.xlsx
+++ b/Iteration 2/Survey/Survey.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="69">
   <si>
     <t>Personal Information</t>
   </si>
@@ -181,39 +181,6 @@
   </si>
   <si>
     <t>Section 2 -Spoken Link Name Referencing</t>
-  </si>
-  <si>
-    <t>Section 3 - Visual Feedback</t>
-  </si>
-  <si>
-    <t>Pop ups</t>
-  </si>
-  <si>
-    <t>Question 3.1</t>
-  </si>
-  <si>
-    <t>Question 3.2</t>
-  </si>
-  <si>
-    <t>Highlighting</t>
-  </si>
-  <si>
-    <t>Section 4 - Visual Feedback</t>
-  </si>
-  <si>
-    <t>Question 4.1</t>
-  </si>
-  <si>
-    <t>Question 4.2</t>
-  </si>
-  <si>
-    <t>Section 5 - Verbal Feedback</t>
-  </si>
-  <si>
-    <t>Question 5.1</t>
-  </si>
-  <si>
-    <t>Question 5.2</t>
   </si>
   <si>
     <t>Birds</t>
@@ -415,7 +382,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -426,7 +393,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -435,16 +401,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -454,7 +414,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -463,18 +422,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -483,7 +438,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -509,12 +463,13 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -809,10 +764,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J99"/>
+  <dimension ref="A1:J87"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" view="pageLayout" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q33" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" showRuler="0" showWhiteSpace="0" view="pageLayout" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N56" sqref="N56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -821,25 +776,25 @@
     <col min="3" max="3" width="4.28515625" customWidth="1"/>
     <col min="5" max="5" width="4.140625" customWidth="1"/>
     <col min="6" max="6" width="9.140625" customWidth="1"/>
-    <col min="7" max="7" width="9.5703125" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" customWidth="1"/>
     <col min="8" max="8" width="9.28515625" customWidth="1"/>
     <col min="9" max="9" width="8.7109375" customWidth="1"/>
     <col min="10" max="10" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18.75">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
     </row>
     <row r="2" spans="1:10" ht="18.75" customHeight="1">
       <c r="A2" s="1" t="s">
@@ -940,15 +895,15 @@
       <c r="J12" s="6"/>
     </row>
     <row r="13" spans="1:10" ht="18.75" customHeight="1">
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="11"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="1" t="s">
@@ -976,7 +931,7 @@
       </c>
     </row>
     <row r="18" spans="2:10">
-      <c r="C18" s="10"/>
+      <c r="C18" s="9"/>
       <c r="D18" t="s">
         <v>28</v>
       </c>
@@ -1076,18 +1031,18 @@
       <c r="J33" s="6"/>
     </row>
     <row r="35" spans="1:10" ht="18.75">
-      <c r="A35" s="27" t="s">
+      <c r="A35" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="B35" s="27"/>
-      <c r="C35" s="28"/>
-      <c r="D35" s="28"/>
-      <c r="E35" s="28"/>
-      <c r="F35" s="28"/>
-      <c r="G35" s="28"/>
-      <c r="H35" s="28"/>
-      <c r="I35" s="28"/>
-      <c r="J35" s="28"/>
+      <c r="B35" s="23"/>
+      <c r="C35" s="24"/>
+      <c r="D35" s="24"/>
+      <c r="E35" s="24"/>
+      <c r="F35" s="24"/>
+      <c r="G35" s="24"/>
+      <c r="H35" s="24"/>
+      <c r="I35" s="24"/>
+      <c r="J35" s="24"/>
     </row>
     <row r="36" spans="1:10">
       <c r="A36" s="1" t="s">
@@ -1105,18 +1060,18 @@
       </c>
     </row>
     <row r="47" spans="1:10" ht="18.75">
-      <c r="A47" s="27" t="s">
+      <c r="A47" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="B47" s="27"/>
-      <c r="C47" s="28"/>
-      <c r="D47" s="28"/>
-      <c r="E47" s="28"/>
-      <c r="F47" s="28"/>
-      <c r="G47" s="28"/>
-      <c r="H47" s="28"/>
-      <c r="I47" s="28"/>
-      <c r="J47" s="28"/>
+      <c r="B47" s="23"/>
+      <c r="C47" s="24"/>
+      <c r="D47" s="24"/>
+      <c r="E47" s="24"/>
+      <c r="F47" s="24"/>
+      <c r="G47" s="24"/>
+      <c r="H47" s="24"/>
+      <c r="I47" s="24"/>
+      <c r="J47" s="24"/>
     </row>
     <row r="48" spans="1:10" ht="18.75">
       <c r="A48" s="3"/>
@@ -1131,696 +1086,483 @@
       <c r="J48" s="4"/>
     </row>
     <row r="49" spans="1:10" ht="15.75">
-      <c r="A49" s="41" t="s">
+      <c r="A49" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="B49" s="41"/>
-      <c r="C49" s="41"/>
-      <c r="D49" s="42" t="s">
+      <c r="B49" s="35"/>
+      <c r="C49" s="35"/>
+      <c r="D49" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="E49" s="43"/>
-      <c r="F49" s="49" t="s">
+      <c r="E49" s="37"/>
+      <c r="F49" s="42" t="s">
         <v>31</v>
       </c>
-      <c r="G49" s="50"/>
-      <c r="H49" s="51"/>
-      <c r="I49" s="55" t="s">
+      <c r="G49" s="43"/>
+      <c r="H49" s="44"/>
+      <c r="I49" s="48" t="s">
         <v>41</v>
       </c>
-      <c r="J49" s="56"/>
+      <c r="J49" s="49"/>
     </row>
     <row r="50" spans="1:10" ht="34.5" customHeight="1">
-      <c r="A50" s="52"/>
-      <c r="B50" s="40"/>
-      <c r="C50" s="40"/>
-      <c r="D50" s="40"/>
-      <c r="E50" s="38"/>
-      <c r="F50" s="15" t="s">
-        <v>77</v>
-      </c>
-      <c r="G50" s="14" t="s">
+      <c r="A50" s="45"/>
+      <c r="B50" s="30"/>
+      <c r="C50" s="31"/>
+      <c r="D50" s="52"/>
+      <c r="E50" s="31"/>
+      <c r="F50" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="G50" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="H50" s="14" t="s">
+      <c r="H50" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="I50" s="53" t="s">
+      <c r="I50" s="46" t="s">
         <v>42</v>
       </c>
-      <c r="J50" s="54"/>
+      <c r="J50" s="47"/>
     </row>
     <row r="51" spans="1:10" s="2" customFormat="1" ht="18.75">
-      <c r="A51" s="46" t="s">
+      <c r="A51" s="39" t="s">
         <v>53</v>
       </c>
-      <c r="B51" s="47"/>
-      <c r="C51" s="47"/>
-      <c r="D51" s="47"/>
-      <c r="E51" s="47"/>
-      <c r="F51" s="47"/>
-      <c r="G51" s="47"/>
-      <c r="H51" s="47"/>
-      <c r="I51" s="47"/>
-      <c r="J51" s="48"/>
+      <c r="B51" s="40"/>
+      <c r="C51" s="40"/>
+      <c r="D51" s="40"/>
+      <c r="E51" s="40"/>
+      <c r="F51" s="40"/>
+      <c r="G51" s="40"/>
+      <c r="H51" s="40"/>
+      <c r="I51" s="40"/>
+      <c r="J51" s="41"/>
     </row>
     <row r="52" spans="1:10">
-      <c r="A52" s="44" t="s">
+      <c r="A52" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="B52" s="45"/>
-      <c r="C52" s="45"/>
-      <c r="D52" s="45"/>
-      <c r="E52" s="45"/>
-      <c r="F52" s="9"/>
-      <c r="G52" s="9"/>
-      <c r="H52" s="9"/>
-      <c r="I52" s="23">
+      <c r="B52" s="33"/>
+      <c r="C52" s="33"/>
+      <c r="D52" s="33"/>
+      <c r="E52" s="33"/>
+      <c r="F52" s="8"/>
+      <c r="G52" s="8"/>
+      <c r="H52" s="8"/>
+      <c r="I52" s="20">
         <v>1</v>
       </c>
-      <c r="J52" s="23">
+      <c r="J52" s="20">
         <v>4</v>
       </c>
     </row>
     <row r="53" spans="1:10">
-      <c r="A53" s="39" t="s">
+      <c r="A53" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="B53" s="40"/>
-      <c r="C53" s="38"/>
-      <c r="D53" s="37"/>
-      <c r="E53" s="38"/>
-      <c r="F53" s="21"/>
-      <c r="G53" s="21"/>
-      <c r="H53" s="21"/>
-      <c r="I53" s="23">
+      <c r="B53" s="30"/>
+      <c r="C53" s="31"/>
+      <c r="D53" s="52"/>
+      <c r="E53" s="31"/>
+      <c r="F53" s="18"/>
+      <c r="G53" s="18"/>
+      <c r="H53" s="18"/>
+      <c r="I53" s="20">
         <v>2</v>
       </c>
-      <c r="J53" s="23">
+      <c r="J53" s="20">
         <v>2</v>
       </c>
     </row>
     <row r="54" spans="1:10">
-      <c r="A54" s="39" t="s">
+      <c r="A54" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="B54" s="40"/>
-      <c r="C54" s="38"/>
-      <c r="D54" s="37"/>
-      <c r="E54" s="38"/>
-      <c r="F54" s="21"/>
-      <c r="G54" s="21"/>
-      <c r="H54" s="21"/>
-      <c r="I54" s="23">
+      <c r="B54" s="30"/>
+      <c r="C54" s="31"/>
+      <c r="D54" s="52"/>
+      <c r="E54" s="31"/>
+      <c r="F54" s="18"/>
+      <c r="G54" s="18"/>
+      <c r="H54" s="18"/>
+      <c r="I54" s="20">
         <v>3</v>
       </c>
-      <c r="J54" s="23">
+      <c r="J54" s="20">
         <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:10">
-      <c r="A55" s="39" t="s">
+      <c r="A55" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="B55" s="40"/>
-      <c r="C55" s="38"/>
-      <c r="D55" s="37"/>
-      <c r="E55" s="38"/>
-      <c r="F55" s="21"/>
-      <c r="G55" s="21"/>
-      <c r="H55" s="21"/>
-      <c r="I55" s="23">
+      <c r="B55" s="30"/>
+      <c r="C55" s="31"/>
+      <c r="D55" s="52"/>
+      <c r="E55" s="31"/>
+      <c r="F55" s="18"/>
+      <c r="G55" s="18"/>
+      <c r="H55" s="18"/>
+      <c r="I55" s="20">
         <v>4</v>
       </c>
-      <c r="J55" s="23">
+      <c r="J55" s="20">
         <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:10">
-      <c r="A56" s="39" t="s">
+      <c r="A56" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="B56" s="40"/>
-      <c r="C56" s="38"/>
-      <c r="D56" s="37"/>
-      <c r="E56" s="38"/>
-      <c r="F56" s="21"/>
-      <c r="G56" s="21"/>
-      <c r="H56" s="21"/>
-      <c r="I56" s="23">
+      <c r="B56" s="30"/>
+      <c r="C56" s="31"/>
+      <c r="D56" s="52"/>
+      <c r="E56" s="31"/>
+      <c r="F56" s="18"/>
+      <c r="G56" s="18"/>
+      <c r="H56" s="18"/>
+      <c r="I56" s="20">
         <v>5</v>
       </c>
-      <c r="J56" s="23">
+      <c r="J56" s="20">
         <v>2</v>
       </c>
     </row>
     <row r="57" spans="1:10" ht="15" customHeight="1">
-      <c r="A57" s="33" t="s">
+      <c r="A57" s="50" t="s">
         <v>54</v>
       </c>
-      <c r="B57" s="34"/>
-      <c r="C57" s="34"/>
-      <c r="D57" s="35"/>
-      <c r="E57" s="35"/>
-      <c r="F57" s="35"/>
-      <c r="G57" s="35"/>
-      <c r="H57" s="35"/>
-      <c r="I57" s="35"/>
-      <c r="J57" s="35"/>
+      <c r="B57" s="51"/>
+      <c r="C57" s="51"/>
+      <c r="D57" s="32"/>
+      <c r="E57" s="32"/>
+      <c r="F57" s="32"/>
+      <c r="G57" s="32"/>
+      <c r="H57" s="32"/>
+      <c r="I57" s="32"/>
+      <c r="J57" s="32"/>
     </row>
     <row r="58" spans="1:10">
-      <c r="A58" s="39" t="s">
+      <c r="A58" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="B58" s="40"/>
-      <c r="C58" s="38"/>
-      <c r="D58" s="37"/>
-      <c r="E58" s="38"/>
-      <c r="F58" s="9"/>
-      <c r="G58" s="9"/>
-      <c r="H58" s="9"/>
-      <c r="I58" s="25" t="s">
-        <v>66</v>
-      </c>
-      <c r="J58" s="25" t="s">
-        <v>71</v>
+      <c r="B58" s="30"/>
+      <c r="C58" s="31"/>
+      <c r="D58" s="52"/>
+      <c r="E58" s="31"/>
+      <c r="F58" s="8"/>
+      <c r="G58" s="8"/>
+      <c r="H58" s="8"/>
+      <c r="I58" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="J58" s="22" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="59" spans="1:10">
-      <c r="A59" s="22" t="s">
+      <c r="A59" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="B59" s="18"/>
-      <c r="C59" s="19"/>
-      <c r="D59" s="24"/>
-      <c r="E59" s="19"/>
-      <c r="F59" s="21"/>
-      <c r="G59" s="21"/>
-      <c r="H59" s="21"/>
-      <c r="I59" s="25" t="s">
+      <c r="B59" s="16"/>
+      <c r="C59" s="17"/>
+      <c r="D59" s="21"/>
+      <c r="E59" s="17"/>
+      <c r="F59" s="18"/>
+      <c r="G59" s="18"/>
+      <c r="H59" s="18"/>
+      <c r="I59" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="J59" s="20" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10">
+      <c r="A60" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="B60" s="16"/>
+      <c r="C60" s="17"/>
+      <c r="D60" s="21"/>
+      <c r="E60" s="17"/>
+      <c r="F60" s="18"/>
+      <c r="G60" s="18"/>
+      <c r="H60" s="18"/>
+      <c r="I60" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="J60" s="20" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" ht="15" customHeight="1">
+      <c r="A61" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="B61" s="16"/>
+      <c r="C61" s="17"/>
+      <c r="D61" s="21"/>
+      <c r="E61" s="17"/>
+      <c r="F61" s="18"/>
+      <c r="G61" s="18"/>
+      <c r="H61" s="18"/>
+      <c r="I61" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="J61" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10">
+      <c r="A62" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="B62" s="30"/>
+      <c r="C62" s="31"/>
+      <c r="D62" s="52"/>
+      <c r="E62" s="31"/>
+      <c r="F62" s="8"/>
+      <c r="G62" s="8"/>
+      <c r="H62" s="8"/>
+      <c r="I62" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="J62" s="22" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" ht="18.75">
+      <c r="A64" s="14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" ht="18.75">
+      <c r="A65" s="3"/>
+      <c r="B65" s="4"/>
+      <c r="C65" s="4"/>
+      <c r="D65" s="4"/>
+      <c r="E65" s="4"/>
+      <c r="F65" s="4"/>
+      <c r="G65" s="4"/>
+      <c r="H65" s="4"/>
+      <c r="I65" s="4"/>
+      <c r="J65" s="4"/>
+    </row>
+    <row r="66" spans="1:10" ht="16.5" customHeight="1">
+      <c r="A66" s="3"/>
+      <c r="B66" s="6"/>
+      <c r="C66" s="6"/>
+      <c r="D66" s="6"/>
+      <c r="E66" s="6"/>
+      <c r="F66" s="6"/>
+      <c r="G66" s="6"/>
+      <c r="H66" s="6"/>
+      <c r="I66" s="6"/>
+      <c r="J66" s="6"/>
+    </row>
+    <row r="67" spans="1:10" ht="18.75">
+      <c r="A67" s="15"/>
+      <c r="B67" s="6"/>
+      <c r="C67" s="6"/>
+      <c r="D67" s="6"/>
+      <c r="E67" s="6"/>
+      <c r="F67" s="6"/>
+      <c r="G67" s="6"/>
+      <c r="H67" s="6"/>
+      <c r="I67" s="6"/>
+      <c r="J67" s="6"/>
+    </row>
+    <row r="68" spans="1:10" ht="18.75">
+      <c r="A68" s="14"/>
+      <c r="B68" s="10"/>
+      <c r="C68" s="10"/>
+      <c r="D68" s="10"/>
+      <c r="E68" s="10"/>
+      <c r="F68" s="10"/>
+      <c r="G68" s="10"/>
+      <c r="H68" s="10"/>
+      <c r="I68" s="10"/>
+      <c r="J68" s="10"/>
+    </row>
+    <row r="69" spans="1:10" ht="18.75">
+      <c r="A69" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B69" s="23"/>
+      <c r="C69" s="24"/>
+      <c r="D69" s="24"/>
+      <c r="E69" s="24"/>
+      <c r="F69" s="24"/>
+      <c r="G69" s="24"/>
+      <c r="H69" s="24"/>
+      <c r="I69" s="24"/>
+      <c r="J69" s="24"/>
+    </row>
+    <row r="70" spans="1:10">
+      <c r="A70" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="J59" s="23" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10">
-      <c r="A60" s="22" t="s">
-        <v>50</v>
-      </c>
-      <c r="B60" s="18"/>
-      <c r="C60" s="19"/>
-      <c r="D60" s="24"/>
-      <c r="E60" s="19"/>
-      <c r="F60" s="21"/>
-      <c r="G60" s="21"/>
-      <c r="H60" s="21"/>
-      <c r="I60" s="25" t="s">
+      <c r="B70" s="10"/>
+      <c r="C70" s="10"/>
+      <c r="D70" s="10"/>
+      <c r="E70" s="10"/>
+      <c r="F70" s="10"/>
+      <c r="G70" s="26"/>
+      <c r="H70" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="I70" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="J70" s="34"/>
+    </row>
+    <row r="71" spans="1:10">
+      <c r="A71" s="10"/>
+      <c r="B71" s="10"/>
+      <c r="C71" s="10"/>
+      <c r="D71" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="E71" s="10"/>
+      <c r="F71" s="10"/>
+      <c r="G71" s="27"/>
+      <c r="H71" s="5"/>
+      <c r="I71" s="33"/>
+      <c r="J71" s="33"/>
+    </row>
+    <row r="72" spans="1:10">
+      <c r="C72" s="10"/>
+      <c r="D72" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="J60" s="23" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10" ht="15" customHeight="1">
-      <c r="A61" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="B61" s="18"/>
-      <c r="C61" s="19"/>
-      <c r="D61" s="24"/>
-      <c r="E61" s="19"/>
-      <c r="F61" s="21"/>
-      <c r="G61" s="21"/>
-      <c r="H61" s="21"/>
-      <c r="I61" s="25" t="s">
-        <v>69</v>
-      </c>
-      <c r="J61" s="23" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10">
-      <c r="A62" s="39" t="s">
-        <v>52</v>
-      </c>
-      <c r="B62" s="40"/>
-      <c r="C62" s="38"/>
-      <c r="D62" s="37"/>
-      <c r="E62" s="38"/>
-      <c r="F62" s="9"/>
-      <c r="G62" s="9"/>
-      <c r="H62" s="9"/>
-      <c r="I62" s="25" t="s">
-        <v>70</v>
-      </c>
-      <c r="J62" s="25" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10" ht="18.75">
-      <c r="A63" s="36" t="s">
-        <v>55</v>
-      </c>
-      <c r="B63" s="35"/>
-      <c r="C63" s="35"/>
-      <c r="D63" s="35"/>
-      <c r="E63" s="35"/>
-      <c r="F63" s="35"/>
-      <c r="G63" s="35"/>
-      <c r="H63" s="35"/>
-      <c r="I63" s="35"/>
-      <c r="J63" s="35"/>
-    </row>
-    <row r="64" spans="1:10" ht="15.75">
-      <c r="A64" s="57" t="s">
-        <v>56</v>
-      </c>
-      <c r="B64" s="58"/>
-      <c r="C64" s="58"/>
-      <c r="D64" s="58"/>
-      <c r="E64" s="58"/>
-      <c r="F64" s="58"/>
-      <c r="G64" s="58"/>
-      <c r="H64" s="58"/>
-      <c r="I64" s="58"/>
-      <c r="J64" s="59"/>
-    </row>
-    <row r="65" spans="1:10">
-      <c r="A65" s="22" t="s">
-        <v>57</v>
-      </c>
-      <c r="B65" s="18"/>
-      <c r="C65" s="18"/>
-      <c r="D65" s="18"/>
-      <c r="E65" s="19"/>
-      <c r="F65" s="21"/>
-      <c r="G65" s="21"/>
-      <c r="H65" s="21"/>
-      <c r="I65" s="23">
-        <v>1</v>
-      </c>
-      <c r="J65" s="23">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10">
-      <c r="A66" s="22" t="s">
-        <v>58</v>
-      </c>
-      <c r="B66" s="18"/>
-      <c r="C66" s="18"/>
-      <c r="D66" s="18"/>
-      <c r="E66" s="19"/>
-      <c r="F66" s="21"/>
-      <c r="G66" s="21"/>
-      <c r="H66" s="21"/>
-      <c r="I66" s="23">
-        <v>2</v>
-      </c>
-      <c r="J66" s="23">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10" ht="18.75">
-      <c r="A67" s="36" t="s">
-        <v>60</v>
-      </c>
-      <c r="B67" s="35"/>
-      <c r="C67" s="35"/>
-      <c r="D67" s="35"/>
-      <c r="E67" s="35"/>
-      <c r="F67" s="35"/>
-      <c r="G67" s="35"/>
-      <c r="H67" s="35"/>
-      <c r="I67" s="35"/>
-      <c r="J67" s="35"/>
-    </row>
-    <row r="68" spans="1:10" ht="15.75">
-      <c r="A68" s="57" t="s">
-        <v>59</v>
-      </c>
-      <c r="B68" s="58"/>
-      <c r="C68" s="58"/>
-      <c r="D68" s="58"/>
-      <c r="E68" s="58"/>
-      <c r="F68" s="58"/>
-      <c r="G68" s="58"/>
-      <c r="H68" s="58"/>
-      <c r="I68" s="58"/>
-      <c r="J68" s="26"/>
-    </row>
-    <row r="69" spans="1:10">
-      <c r="A69" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="B69" s="18"/>
-      <c r="C69" s="18"/>
-      <c r="D69" s="18"/>
-      <c r="E69" s="19"/>
-      <c r="F69" s="21"/>
-      <c r="G69" s="21"/>
-      <c r="H69" s="21"/>
-      <c r="I69" s="23">
-        <v>1</v>
-      </c>
-      <c r="J69" s="23">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="70" spans="1:10">
-      <c r="A70" s="39" t="s">
-        <v>62</v>
-      </c>
-      <c r="B70" s="40"/>
-      <c r="C70" s="40"/>
-      <c r="D70" s="40"/>
-      <c r="E70" s="38"/>
-      <c r="F70" s="9"/>
-      <c r="G70" s="9"/>
-      <c r="H70" s="9"/>
-      <c r="I70" s="23">
-        <v>2</v>
-      </c>
-      <c r="J70" s="23">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="71" spans="1:10" ht="18.75">
-      <c r="A71" s="36" t="s">
-        <v>63</v>
-      </c>
-      <c r="B71" s="35"/>
-      <c r="C71" s="35"/>
-      <c r="D71" s="35"/>
-      <c r="E71" s="35"/>
-      <c r="F71" s="35"/>
-      <c r="G71" s="35"/>
-      <c r="H71" s="35"/>
-      <c r="I71" s="35"/>
-      <c r="J71" s="35"/>
-    </row>
-    <row r="72" spans="1:10">
-      <c r="A72" s="39" t="s">
-        <v>64</v>
-      </c>
-      <c r="B72" s="40"/>
-      <c r="C72" s="38"/>
-      <c r="D72" s="45"/>
-      <c r="E72" s="45"/>
-      <c r="F72" s="9"/>
-      <c r="G72" s="8"/>
-      <c r="H72" s="9"/>
-      <c r="I72" s="20">
-        <v>1</v>
-      </c>
-      <c r="J72" s="23">
-        <v>4</v>
-      </c>
+      <c r="E72" s="1"/>
+      <c r="H72" s="5"/>
+      <c r="I72" s="33"/>
+      <c r="J72" s="33"/>
     </row>
     <row r="73" spans="1:10">
-      <c r="A73" s="39" t="s">
-        <v>65</v>
-      </c>
-      <c r="B73" s="40"/>
-      <c r="C73" s="38"/>
-      <c r="D73" s="45"/>
-      <c r="E73" s="45"/>
-      <c r="F73" s="9"/>
-      <c r="G73" s="9"/>
-      <c r="H73" s="9"/>
-      <c r="I73" s="20">
-        <v>2</v>
-      </c>
-      <c r="J73" s="23">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="75" spans="1:10" ht="18.75">
-      <c r="A75" s="16" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="76" spans="1:10" ht="18.75">
-      <c r="A76" s="3"/>
+      <c r="C73" s="10"/>
+      <c r="D73" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E73" s="1"/>
+      <c r="H73" s="5"/>
+      <c r="I73" s="33"/>
+      <c r="J73" s="33"/>
+    </row>
+    <row r="75" spans="1:10">
+      <c r="A75" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I75" s="10"/>
+      <c r="J75" s="10"/>
+    </row>
+    <row r="76" spans="1:10" ht="18.75" customHeight="1">
+      <c r="A76" s="4"/>
       <c r="B76" s="4"/>
       <c r="C76" s="4"/>
-      <c r="D76" s="4"/>
-      <c r="E76" s="4"/>
+      <c r="D76" s="12"/>
+      <c r="E76" s="12"/>
       <c r="F76" s="4"/>
       <c r="G76" s="4"/>
       <c r="H76" s="4"/>
       <c r="I76" s="4"/>
       <c r="J76" s="4"/>
     </row>
-    <row r="77" spans="1:10" ht="16.5" customHeight="1">
-      <c r="A77" s="3"/>
+    <row r="77" spans="1:10" ht="18.75" customHeight="1">
+      <c r="A77" s="6"/>
       <c r="B77" s="6"/>
       <c r="C77" s="6"/>
-      <c r="D77" s="6"/>
-      <c r="E77" s="6"/>
+      <c r="D77" s="11"/>
+      <c r="E77" s="11"/>
       <c r="F77" s="6"/>
       <c r="G77" s="6"/>
       <c r="H77" s="6"/>
       <c r="I77" s="6"/>
       <c r="J77" s="6"/>
     </row>
-    <row r="78" spans="1:10" ht="18.75">
-      <c r="A78" s="17"/>
+    <row r="78" spans="1:10" ht="18.75" customHeight="1">
+      <c r="A78" s="6"/>
       <c r="B78" s="6"/>
       <c r="C78" s="6"/>
-      <c r="D78" s="6"/>
-      <c r="E78" s="6"/>
+      <c r="D78" s="11"/>
+      <c r="E78" s="11"/>
       <c r="F78" s="6"/>
       <c r="G78" s="6"/>
       <c r="H78" s="6"/>
       <c r="I78" s="6"/>
       <c r="J78" s="6"/>
     </row>
-    <row r="79" spans="1:10" ht="18.75">
-      <c r="A79" s="16"/>
-      <c r="B79" s="11"/>
-      <c r="C79" s="11"/>
-      <c r="D79" s="11"/>
-      <c r="E79" s="11"/>
-      <c r="F79" s="11"/>
-      <c r="G79" s="11"/>
-      <c r="H79" s="11"/>
-      <c r="I79" s="11"/>
-      <c r="J79" s="11"/>
-    </row>
-    <row r="80" spans="1:10" ht="18.75">
-      <c r="A80" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="B80" s="27"/>
-      <c r="C80" s="28"/>
-      <c r="D80" s="28"/>
-      <c r="E80" s="28"/>
-      <c r="F80" s="28"/>
-      <c r="G80" s="28"/>
-      <c r="H80" s="28"/>
-      <c r="I80" s="28"/>
-      <c r="J80" s="28"/>
+    <row r="79" spans="1:10">
+      <c r="A79" s="10"/>
+      <c r="B79" s="10"/>
+      <c r="C79" s="10"/>
+      <c r="D79" s="25"/>
+      <c r="E79" s="25"/>
+      <c r="F79" s="10"/>
+      <c r="G79" s="10"/>
+      <c r="H79" s="10"/>
+      <c r="I79" s="10"/>
+      <c r="J79" s="10"/>
     </row>
     <row r="81" spans="1:10">
-      <c r="A81" s="29" t="s">
-        <v>78</v>
-      </c>
-      <c r="B81" s="11"/>
-      <c r="C81" s="11"/>
-      <c r="D81" s="11"/>
-      <c r="E81" s="11"/>
-      <c r="F81" s="11"/>
-      <c r="G81" s="30"/>
-      <c r="H81" s="32" t="s">
-        <v>32</v>
-      </c>
-      <c r="I81" s="60" t="s">
-        <v>33</v>
-      </c>
-      <c r="J81" s="60"/>
+      <c r="A81" s="1" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="82" spans="1:10">
-      <c r="A82" s="11"/>
-      <c r="B82" s="11"/>
-      <c r="C82" s="11"/>
-      <c r="D82" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="E82" s="11"/>
-      <c r="F82" s="11"/>
-      <c r="G82" s="31"/>
-      <c r="H82" s="5"/>
-      <c r="I82" s="45"/>
-      <c r="J82" s="45"/>
-    </row>
-    <row r="83" spans="1:10">
-      <c r="C83" s="11"/>
-      <c r="D83" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E83" s="1"/>
-      <c r="H83" s="5"/>
-      <c r="I83" s="45"/>
-      <c r="J83" s="45"/>
+      <c r="C82" s="5"/>
+      <c r="D82" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E82" s="5"/>
+      <c r="F82" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="84" spans="1:10">
-      <c r="C84" s="11"/>
-      <c r="D84" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E84" s="1"/>
-      <c r="H84" s="5"/>
-      <c r="I84" s="45"/>
-      <c r="J84" s="45"/>
-    </row>
-    <row r="86" spans="1:10">
-      <c r="A86" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="I86" s="11"/>
-      <c r="J86" s="11"/>
+      <c r="B84" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" ht="18.75" customHeight="1">
+      <c r="C85" s="4"/>
+      <c r="D85" s="4"/>
+      <c r="E85" s="4"/>
+      <c r="F85" s="4"/>
+      <c r="G85" s="4"/>
+      <c r="H85" s="4"/>
+      <c r="I85" s="4"/>
+      <c r="J85" s="4"/>
+    </row>
+    <row r="86" spans="1:10" ht="18.75" customHeight="1">
+      <c r="C86" s="6"/>
+      <c r="D86" s="6"/>
+      <c r="E86" s="6"/>
+      <c r="F86" s="6"/>
+      <c r="G86" s="6"/>
+      <c r="H86" s="6"/>
+      <c r="I86" s="6"/>
+      <c r="J86" s="6"/>
     </row>
     <row r="87" spans="1:10" ht="18.75" customHeight="1">
-      <c r="A87" s="4"/>
-      <c r="B87" s="4"/>
-      <c r="C87" s="4"/>
-      <c r="D87" s="13"/>
-      <c r="E87" s="13"/>
-      <c r="F87" s="4"/>
-      <c r="G87" s="4"/>
-      <c r="H87" s="4"/>
-      <c r="I87" s="4"/>
-      <c r="J87" s="4"/>
-    </row>
-    <row r="88" spans="1:10" ht="18.75" customHeight="1">
-      <c r="A88" s="6"/>
-      <c r="B88" s="6"/>
-      <c r="C88" s="6"/>
-      <c r="D88" s="12"/>
-      <c r="E88" s="12"/>
-      <c r="F88" s="6"/>
-      <c r="G88" s="6"/>
-      <c r="H88" s="6"/>
-      <c r="I88" s="6"/>
-      <c r="J88" s="6"/>
-    </row>
-    <row r="89" spans="1:10" ht="18.75" customHeight="1">
-      <c r="A89" s="6"/>
-      <c r="B89" s="6"/>
-      <c r="C89" s="6"/>
-      <c r="D89" s="12"/>
-      <c r="E89" s="12"/>
-      <c r="F89" s="6"/>
-      <c r="G89" s="6"/>
-      <c r="H89" s="6"/>
-      <c r="I89" s="6"/>
-      <c r="J89" s="6"/>
-    </row>
-    <row r="90" spans="1:10">
-      <c r="A90" s="11"/>
-      <c r="B90" s="11"/>
-      <c r="C90" s="11"/>
-      <c r="D90" s="29"/>
-      <c r="E90" s="29"/>
-      <c r="F90" s="11"/>
-      <c r="G90" s="11"/>
-      <c r="H90" s="11"/>
-      <c r="I90" s="11"/>
-      <c r="J90" s="11"/>
-    </row>
-    <row r="91" spans="1:10">
-      <c r="A91" s="11"/>
-      <c r="B91" s="11"/>
-      <c r="C91" s="11"/>
-      <c r="D91" s="29"/>
-      <c r="E91" s="29"/>
-      <c r="F91" s="11"/>
-      <c r="G91" s="11"/>
-      <c r="H91" s="11"/>
-      <c r="I91" s="11"/>
-      <c r="J91" s="11"/>
-    </row>
-    <row r="93" spans="1:10">
-      <c r="A93" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="94" spans="1:10">
-      <c r="C94" s="5"/>
-      <c r="D94" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E94" s="5"/>
-      <c r="F94" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="96" spans="1:10">
-      <c r="B96" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C96" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="97" spans="3:10" ht="18.75" customHeight="1">
-      <c r="C97" s="4"/>
-      <c r="D97" s="4"/>
-      <c r="E97" s="4"/>
-      <c r="F97" s="4"/>
-      <c r="G97" s="4"/>
-      <c r="H97" s="4"/>
-      <c r="I97" s="4"/>
-      <c r="J97" s="4"/>
-    </row>
-    <row r="98" spans="3:10" ht="18.75" customHeight="1">
-      <c r="C98" s="6"/>
-      <c r="D98" s="6"/>
-      <c r="E98" s="6"/>
-      <c r="F98" s="6"/>
-      <c r="G98" s="6"/>
-      <c r="H98" s="6"/>
-      <c r="I98" s="6"/>
-      <c r="J98" s="6"/>
-    </row>
-    <row r="99" spans="3:10" ht="18.75" customHeight="1">
-      <c r="C99" s="6"/>
-      <c r="D99" s="6"/>
-      <c r="E99" s="6"/>
-      <c r="F99" s="6"/>
-      <c r="G99" s="6"/>
-      <c r="H99" s="6"/>
-      <c r="I99" s="6"/>
-      <c r="J99" s="6"/>
+      <c r="C87" s="6"/>
+      <c r="D87" s="6"/>
+      <c r="E87" s="6"/>
+      <c r="F87" s="6"/>
+      <c r="G87" s="6"/>
+      <c r="H87" s="6"/>
+      <c r="I87" s="6"/>
+      <c r="J87" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="36">
-    <mergeCell ref="A70:E70"/>
-    <mergeCell ref="A67:J67"/>
-    <mergeCell ref="A64:J64"/>
-    <mergeCell ref="A68:I68"/>
-    <mergeCell ref="I84:J84"/>
-    <mergeCell ref="I81:J81"/>
-    <mergeCell ref="I82:J82"/>
-    <mergeCell ref="A71:J71"/>
-    <mergeCell ref="D72:E72"/>
-    <mergeCell ref="A72:C72"/>
-    <mergeCell ref="D73:E73"/>
-    <mergeCell ref="A73:C73"/>
-    <mergeCell ref="I83:J83"/>
-    <mergeCell ref="A49:C49"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="A52:C52"/>
-    <mergeCell ref="A51:J51"/>
-    <mergeCell ref="F49:H49"/>
-    <mergeCell ref="A50:E50"/>
-    <mergeCell ref="I50:J50"/>
-    <mergeCell ref="I49:J49"/>
-    <mergeCell ref="D52:E52"/>
+  <mergeCells count="27">
     <mergeCell ref="A57:J57"/>
-    <mergeCell ref="A63:J63"/>
     <mergeCell ref="D56:E56"/>
     <mergeCell ref="A53:C53"/>
     <mergeCell ref="A54:C54"/>
@@ -1833,6 +1575,20 @@
     <mergeCell ref="A62:C62"/>
     <mergeCell ref="D58:E58"/>
     <mergeCell ref="D62:E62"/>
+    <mergeCell ref="A49:C49"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="A52:C52"/>
+    <mergeCell ref="A51:J51"/>
+    <mergeCell ref="F49:H49"/>
+    <mergeCell ref="I50:J50"/>
+    <mergeCell ref="I49:J49"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="A50:C50"/>
+    <mergeCell ref="I73:J73"/>
+    <mergeCell ref="I70:J70"/>
+    <mergeCell ref="I71:J71"/>
+    <mergeCell ref="I72:J72"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>